<commit_message>
Change UNDER exception logic to show current allocation period
Modified AllocationAnalyzer to show when employees are currently
allocated (within query window) rather than when they'll be free.
This helps identify when people will become available for new work.

For example, if Levin is allocated until 2026-02-28:
- Old behavior: Exception from 2026-03-01 to 2026-04-18 (free period)
- New behavior: Exception from 2026-01-18 to 2026-02-28 (busy period)

The exception indicates "this person is busy until [end_date],
then will need new allocation."

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/exceptions.xlsx
+++ b/data/exceptions.xlsx
@@ -432,7 +432,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Galandor Moshe Yakov</v>
+        <v>Chen Noam</v>
       </c>
       <c r="B2" t="str">
         <v>UNDER</v>
@@ -441,10 +441,10 @@
         <v>2026-01-18</v>
       </c>
       <c r="D2" t="str">
-        <v>2026-04-18</v>
+        <v>2026-02-15</v>
       </c>
       <c r="E2">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F2" t="str">
         <v>None</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Noiman Yehuda</v>
+        <v>Galandor Moshe Yakov</v>
       </c>
       <c r="B3" t="str">
         <v>UNDER</v>
@@ -461,10 +461,10 @@
         <v>2026-01-18</v>
       </c>
       <c r="D3" t="str">
-        <v>2026-01-31</v>
+        <v>2026-04-18</v>
       </c>
       <c r="E3">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="F3" t="str">
         <v>None</v>
@@ -472,7 +472,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Itzhaki Yair</v>
+        <v>Meir Zipora</v>
       </c>
       <c r="B4" t="str">
         <v>UNDER</v>
@@ -481,10 +481,10 @@
         <v>2026-01-18</v>
       </c>
       <c r="D4" t="str">
-        <v>2026-04-18</v>
+        <v>2026-02-28</v>
       </c>
       <c r="E4">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="F4" t="str">
         <v>None</v>
@@ -498,13 +498,13 @@
         <v>UNDER</v>
       </c>
       <c r="C5" t="str">
-        <v>2026-02-01</v>
+        <v>2026-01-18</v>
       </c>
       <c r="D5" t="str">
-        <v>2026-04-18</v>
+        <v>2026-01-31</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F5" t="str">
         <v>None</v>
@@ -512,16 +512,16 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Chen Noam</v>
+        <v>Noiman Yehuda</v>
       </c>
       <c r="B6" t="str">
         <v>UNDER</v>
       </c>
       <c r="C6" t="str">
-        <v>2026-02-16</v>
+        <v>2026-01-18</v>
       </c>
       <c r="D6" t="str">
-        <v>2026-04-18</v>
+        <v>2026-01-31</v>
       </c>
       <c r="E6">
         <v>100</v>
@@ -532,19 +532,19 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Meir Zipora</v>
+        <v>Weingarten Ayala</v>
       </c>
       <c r="B7" t="str">
         <v>UNDER</v>
       </c>
       <c r="C7" t="str">
-        <v>2026-03-01</v>
+        <v>2026-01-18</v>
       </c>
       <c r="D7" t="str">
-        <v>2026-04-18</v>
+        <v>2026-02-28</v>
       </c>
       <c r="E7">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F7" t="str">
         <v>None</v>
@@ -552,19 +552,19 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Weingarten Ayala</v>
+        <v>Itzhaki Yair</v>
       </c>
       <c r="B8" t="str">
         <v>UNDER</v>
       </c>
       <c r="C8" t="str">
-        <v>2026-03-01</v>
+        <v>2026-01-18</v>
       </c>
       <c r="D8" t="str">
         <v>2026-04-18</v>
       </c>
       <c r="E8">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F8" t="str">
         <v>None</v>
@@ -572,16 +572,16 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Levin Yanir</v>
+        <v>Peretz Yehonathan</v>
       </c>
       <c r="B9" t="str">
         <v>UNDER</v>
       </c>
       <c r="C9" t="str">
-        <v>2026-03-01</v>
+        <v>2026-01-18</v>
       </c>
       <c r="D9" t="str">
-        <v>2026-04-18</v>
+        <v>2026-03-31</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -592,16 +592,16 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Halevy Maor</v>
+        <v>Levin Yanir</v>
       </c>
       <c r="B10" t="str">
         <v>UNDER</v>
       </c>
       <c r="C10" t="str">
-        <v>2026-03-01</v>
+        <v>2026-01-18</v>
       </c>
       <c r="D10" t="str">
-        <v>2026-04-18</v>
+        <v>2026-02-28</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -612,16 +612,16 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Peretz Yehonathan</v>
+        <v>Halevy Maor</v>
       </c>
       <c r="B11" t="str">
         <v>UNDER</v>
       </c>
       <c r="C11" t="str">
-        <v>2026-04-01</v>
+        <v>2026-01-18</v>
       </c>
       <c r="D11" t="str">
-        <v>2026-04-18</v>
+        <v>2026-02-28</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -638,10 +638,10 @@
         <v>UNDER</v>
       </c>
       <c r="C12" t="str">
-        <v>2026-04-01</v>
+        <v>2026-01-18</v>
       </c>
       <c r="D12" t="str">
-        <v>2026-04-18</v>
+        <v>2026-03-31</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -658,10 +658,10 @@
         <v>UNDER</v>
       </c>
       <c r="C13" t="str">
-        <v>2026-04-01</v>
+        <v>2026-01-18</v>
       </c>
       <c r="D13" t="str">
-        <v>2026-04-18</v>
+        <v>2026-03-31</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -678,10 +678,10 @@
         <v>UNDER</v>
       </c>
       <c r="C14" t="str">
-        <v>2026-04-01</v>
+        <v>2026-01-18</v>
       </c>
       <c r="D14" t="str">
-        <v>2026-04-18</v>
+        <v>2026-03-31</v>
       </c>
       <c r="E14">
         <v>100</v>

</xml_diff>

<commit_message>
Add source projects/clients to UNDER exceptions
Modified AllocationAnalyzer to populate source_projects_or_clients
for UNDER exceptions that show current allocation periods.

Logic:
- Only transforms exceptions where employee was fully allocated
  (total allocation >= FTE, within 1% tolerance)
- Partial allocations (like 50% when FTE is 100%) are not transformed
- Shows which projects/clients the employee is currently working on

Example: Levin allocated 100% to "Speedata Ltd" until 2026-02-28
- Exception shows: 2026-01-18 to 2026-02-28 (current allocation)
- Source: ["Speedata Ltd"]

Updated exceptions.xlsx with source information.

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/exceptions.xlsx
+++ b/data/exceptions.xlsx
@@ -447,7 +447,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="str">
-        <v>None</v>
+        <v>Sightec (Israel) Ltd.</v>
       </c>
     </row>
     <row r="3">
@@ -487,7 +487,7 @@
         <v>87</v>
       </c>
       <c r="F4" t="str">
-        <v>None</v>
+        <v>BioXtreme Ltd.</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +512,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Noiman Yehuda</v>
+        <v>Weingarten Ayala</v>
       </c>
       <c r="B6" t="str">
         <v>UNDER</v>
@@ -521,18 +521,18 @@
         <v>2026-01-18</v>
       </c>
       <c r="D6" t="str">
-        <v>2026-01-31</v>
+        <v>2026-02-28</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="F6" t="str">
-        <v>None</v>
+        <v>Arad Technologies Ltd.</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Weingarten Ayala</v>
+        <v>Itzhaki Yair</v>
       </c>
       <c r="B7" t="str">
         <v>UNDER</v>
@@ -541,10 +541,10 @@
         <v>2026-01-18</v>
       </c>
       <c r="D7" t="str">
-        <v>2026-02-28</v>
+        <v>2026-04-18</v>
       </c>
       <c r="E7">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F7" t="str">
         <v>None</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Itzhaki Yair</v>
+        <v>Peretz Yehonathan</v>
       </c>
       <c r="B8" t="str">
         <v>UNDER</v>
@@ -561,18 +561,18 @@
         <v>2026-01-18</v>
       </c>
       <c r="D8" t="str">
-        <v>2026-04-18</v>
+        <v>2026-03-31</v>
       </c>
       <c r="E8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F8" t="str">
-        <v>None</v>
+        <v>Red Sea</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Peretz Yehonathan</v>
+        <v>Levin Yanir</v>
       </c>
       <c r="B9" t="str">
         <v>UNDER</v>
@@ -581,18 +581,18 @@
         <v>2026-01-18</v>
       </c>
       <c r="D9" t="str">
-        <v>2026-03-31</v>
+        <v>2026-02-28</v>
       </c>
       <c r="E9">
         <v>100</v>
       </c>
       <c r="F9" t="str">
-        <v>None</v>
+        <v>Speedata Ltd</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Levin Yanir</v>
+        <v>Halevy Maor</v>
       </c>
       <c r="B10" t="str">
         <v>UNDER</v>
@@ -607,12 +607,12 @@
         <v>100</v>
       </c>
       <c r="F10" t="str">
-        <v>None</v>
+        <v>Rav Bariach Locks Products LTD.</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Halevy Maor</v>
+        <v>Cohen Aharon</v>
       </c>
       <c r="B11" t="str">
         <v>UNDER</v>
@@ -621,18 +621,18 @@
         <v>2026-01-18</v>
       </c>
       <c r="D11" t="str">
-        <v>2026-02-28</v>
+        <v>2026-03-31</v>
       </c>
       <c r="E11">
         <v>100</v>
       </c>
       <c r="F11" t="str">
-        <v>None</v>
+        <v>Aquestia Ltd.</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Cohen Aharon</v>
+        <v>Pruzanski Yossi</v>
       </c>
       <c r="B12" t="str">
         <v>UNDER</v>
@@ -647,12 +647,12 @@
         <v>100</v>
       </c>
       <c r="F12" t="str">
-        <v>None</v>
+        <v>Maytronics Ltd.</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Pruzanski Yossi</v>
+        <v>Morgenstern Elisheva</v>
       </c>
       <c r="B13" t="str">
         <v>UNDER</v>
@@ -667,21 +667,21 @@
         <v>100</v>
       </c>
       <c r="F13" t="str">
-        <v>None</v>
+        <v>Red Sea</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Morgenstern Elisheva</v>
+        <v>Noiman Yehuda</v>
       </c>
       <c r="B14" t="str">
         <v>UNDER</v>
       </c>
       <c r="C14" t="str">
-        <v>2026-01-18</v>
+        <v>2026-02-01</v>
       </c>
       <c r="D14" t="str">
-        <v>2026-03-31</v>
+        <v>2026-04-18</v>
       </c>
       <c r="E14">
         <v>100</v>

</xml_diff>